<commit_message>
Reading fingerprints from the database
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>b'AQAABLSbMQn8sUgeIbe8AMEE'</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,6 +461,9 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -466,6 +472,9 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -496,6 +505,9 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -503,6 +515,9 @@
       </c>
       <c r="B10" t="s">
         <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>